<commit_message>
:sparkles: Ajout indicateurs fin sprint et correctifs
</commit_message>
<xml_diff>
--- a/Sprint2/IndicateursFin.xlsx
+++ b/Sprint2/IndicateursFin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thom5\Documents\BUT3\QualDev\BUT3_QUALDEV_GROUPE3\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FD11FD-69D2-416A-96B6-E1EA30457284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4193CA-4DCC-4B4C-956D-2D61F41924FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,7 +355,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -368,7 +368,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -376,7 +376,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>143</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>